<commit_message>
Migrated BookStore and Account tests to Playwright with Excel DataProvider support
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/AppData.xlsx
+++ b/src/test/resources/testdata/AppData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8400" activeTab="4"/>
+    <workbookView windowWidth="23040" windowHeight="8400" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="AddMultipleRecords" sheetId="9" r:id="rId3"/>
     <sheet name="NewUserRegistration" sheetId="10" r:id="rId4"/>
     <sheet name="AddRecords" sheetId="11" r:id="rId5"/>
+    <sheet name="BookDetails" sheetId="12" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="71">
   <si>
     <t>Valid Username</t>
   </si>
@@ -190,6 +191,60 @@
   </si>
   <si>
     <t>adiCh#212$</t>
+  </si>
+  <si>
+    <t>ISBN</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>SubTitle</t>
+  </si>
+  <si>
+    <t>Author</t>
+  </si>
+  <si>
+    <t>PublishDate</t>
+  </si>
+  <si>
+    <t>Publisher</t>
+  </si>
+  <si>
+    <t>Pages</t>
+  </si>
+  <si>
+    <t>9781449325862</t>
+  </si>
+  <si>
+    <t>Git Pocket Guide</t>
+  </si>
+  <si>
+    <t>A Working Introduction</t>
+  </si>
+  <si>
+    <t>Richard E. Silverman</t>
+  </si>
+  <si>
+    <t>2020-06-04T08:48:39.000Z</t>
+  </si>
+  <si>
+    <t>O'Reilly Media</t>
+  </si>
+  <si>
+    <t>9781491950296</t>
+  </si>
+  <si>
+    <t>Programming JavaScript Applications</t>
+  </si>
+  <si>
+    <t>Robust Web Architecture with Node, HTML5, and Modern JS Libraries</t>
+  </si>
+  <si>
+    <t>Eric Elliott</t>
+  </si>
+  <si>
+    <t>2014-07-01T00:00:00.000Z</t>
   </si>
 </sst>
 </file>
@@ -213,6 +268,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -223,13 +285,6 @@
       <color rgb="FF212529"/>
       <name val="Segoe UI"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -368,7 +423,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -377,6 +432,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF757171"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -562,12 +623,40 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -682,19 +771,19 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -703,7 +792,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -715,129 +804,132 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="19" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="19" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="19" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="19" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="19"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="19"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1201,16 +1293,16 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.9" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1288,22 +1380,22 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="5"/>
   <sheetData>
     <row r="1" ht="15.9" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1314,16 +1406,16 @@
       <c r="B2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="6">
         <v>28</v>
       </c>
       <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1348,22 +1440,22 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.9" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1371,20 +1463,20 @@
       <c r="A2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D2" t="str">
         <f>_xlfn.CONCAT(A2,".",B2,"@gmail.com")</f>
         <v>Anil.Sharma@gmail.com</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1392,20 +1484,20 @@
       <c r="A3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D3" t="str">
         <f>_xlfn.CONCAT(A3,".",B3,"@gmail.com")</f>
         <v>Sneha.Gupta@gmail.com</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1413,827 +1505,729 @@
       <c r="A4" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="6" t="s">
         <v>43</v>
       </c>
       <c r="D4" t="str">
         <f>_xlfn.CONCAT(A4,".",B4,"@gmail.com")</f>
         <v>Rohan.Sen@gmail.com</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" ht="15" spans="1:6">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D5" t="str">
         <f>_xlfn.CONCAT(A5,".",B5,"@gmail.com")</f>
         <v>Aditi.Chakrabotry@gmail.com</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="6" ht="15" spans="1:6">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="3"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" ht="15" spans="1:6">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4"/>
-      <c r="D7"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="3"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" ht="15" spans="1:6">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
-      <c r="D8"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="3"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" ht="15" spans="1:6">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="3"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" ht="15" spans="1:6">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4"/>
-      <c r="D10"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="3"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" ht="15" spans="1:6">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="4"/>
-      <c r="D11"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="3"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" ht="15" spans="1:6">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="3"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" ht="15" spans="1:6">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="4"/>
-      <c r="D13"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="3"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" ht="15" spans="1:6">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="4"/>
-      <c r="D14"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="3"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" ht="15" spans="1:6">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="3"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="5"/>
     </row>
     <row r="16" ht="15" spans="1:6">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="4"/>
-      <c r="D16"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="3"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="5"/>
     </row>
     <row r="17" ht="15" spans="1:6">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="4"/>
-      <c r="D17"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="3"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" ht="15" spans="1:6">
-      <c r="A18" s="3"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="3"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="5"/>
     </row>
     <row r="19" ht="15" spans="1:6">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="4"/>
-      <c r="D19"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="3"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="5"/>
     </row>
     <row r="20" ht="15" spans="1:6">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="4"/>
-      <c r="D20"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="3"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="5"/>
     </row>
     <row r="21" ht="15" spans="1:6">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="3"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="5"/>
     </row>
     <row r="22" ht="15" spans="1:6">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="4"/>
-      <c r="D22"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="3"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="5"/>
     </row>
     <row r="23" ht="15" spans="1:6">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="4"/>
-      <c r="D23"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="3"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="5"/>
     </row>
     <row r="24" ht="15" spans="1:6">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="3"/>
+      <c r="A24" s="5"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="5"/>
     </row>
     <row r="25" ht="15" spans="1:6">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="4"/>
-      <c r="D25"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="3"/>
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="5"/>
     </row>
     <row r="26" ht="15" spans="1:6">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="4"/>
-      <c r="D26"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="3"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="5"/>
     </row>
     <row r="27" ht="15" spans="1:6">
-      <c r="A27" s="3"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="3"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="5"/>
     </row>
     <row r="28" ht="15" spans="1:6">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="4"/>
-      <c r="D28"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="3"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="6"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="5"/>
     </row>
     <row r="29" ht="15" spans="1:6">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="4"/>
-      <c r="D29"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="3"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="6"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="5"/>
     </row>
     <row r="30" ht="15" spans="1:6">
-      <c r="A30" s="3"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="3"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="5"/>
     </row>
     <row r="31" ht="15" spans="1:6">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="4"/>
-      <c r="D31"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="3"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="6"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="5"/>
     </row>
     <row r="32" ht="15" spans="1:6">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="4"/>
-      <c r="D32"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="3"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="6"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="5"/>
     </row>
     <row r="33" ht="15" spans="1:6">
-      <c r="A33" s="3"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="3"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="5"/>
     </row>
     <row r="34" ht="15" spans="1:6">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="4"/>
-      <c r="D34"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="3"/>
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="6"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="5"/>
     </row>
     <row r="35" ht="15" spans="1:6">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="4"/>
-      <c r="D35"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="3"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="6"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="5"/>
     </row>
     <row r="36" ht="15" spans="1:6">
-      <c r="A36" s="3"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="3"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="5"/>
     </row>
     <row r="37" ht="15" spans="1:6">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="4"/>
-      <c r="D37"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="3"/>
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="6"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="5"/>
     </row>
     <row r="38" ht="15" spans="1:6">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="4"/>
-      <c r="D38"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="3"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="6"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="5"/>
     </row>
     <row r="39" ht="15" spans="1:6">
-      <c r="A39" s="3"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="3"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="5"/>
     </row>
     <row r="40" ht="15" spans="1:6">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="4"/>
-      <c r="D40"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="3"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="6"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="5"/>
     </row>
     <row r="41" ht="15" spans="1:6">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="4"/>
-      <c r="D41"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="3"/>
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="6"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="5"/>
     </row>
     <row r="42" ht="15" spans="1:6">
-      <c r="A42" s="3"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="3"/>
+      <c r="A42" s="5"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="5"/>
     </row>
     <row r="43" ht="15" spans="1:6">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="4"/>
-      <c r="D43"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="3"/>
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="6"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="5"/>
     </row>
     <row r="44" ht="15" spans="1:6">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="4"/>
-      <c r="D44"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="3"/>
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="6"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="5"/>
     </row>
     <row r="45" ht="15" spans="1:6">
-      <c r="A45" s="3"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
-      <c r="D45"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="3"/>
+      <c r="A45" s="5"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="5"/>
     </row>
     <row r="46" ht="15" spans="1:6">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="4"/>
-      <c r="D46"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="3"/>
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="6"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="5"/>
     </row>
     <row r="47" ht="15" spans="1:6">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="4"/>
-      <c r="D47"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="3"/>
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="6"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="5"/>
     </row>
     <row r="48" ht="15" spans="1:6">
-      <c r="A48" s="3"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="3"/>
+      <c r="A48" s="5"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="5"/>
     </row>
     <row r="49" ht="15" spans="1:6">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="4"/>
-      <c r="D49"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="3"/>
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="6"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="5"/>
     </row>
     <row r="50" ht="15" spans="1:6">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="4"/>
-      <c r="D50"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="3"/>
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="6"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="5"/>
     </row>
     <row r="51" ht="15" spans="1:6">
-      <c r="A51" s="3"/>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="3"/>
+      <c r="A51" s="5"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="5"/>
     </row>
     <row r="52" ht="15" spans="1:6">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="4"/>
-      <c r="D52"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="3"/>
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="6"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="5"/>
     </row>
     <row r="53" ht="15" spans="1:6">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="4"/>
-      <c r="D53"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="3"/>
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="6"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="5"/>
     </row>
     <row r="54" ht="15" spans="1:6">
-      <c r="A54" s="3"/>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-      <c r="D54"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="3"/>
+      <c r="A54" s="5"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="5"/>
     </row>
     <row r="55" ht="15" spans="1:6">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="4"/>
-      <c r="D55"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="3"/>
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="6"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="5"/>
     </row>
     <row r="56" ht="15" spans="1:6">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="4"/>
-      <c r="D56"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="3"/>
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="6"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="5"/>
     </row>
     <row r="57" ht="15" spans="1:6">
-      <c r="A57" s="3"/>
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-      <c r="D57"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="3"/>
+      <c r="A57" s="5"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="5"/>
     </row>
     <row r="58" ht="15" spans="1:6">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="4"/>
-      <c r="D58"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="3"/>
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="6"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="5"/>
     </row>
     <row r="59" ht="15" spans="1:6">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="4"/>
-      <c r="D59"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="3"/>
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="6"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="5"/>
     </row>
     <row r="60" ht="15" spans="1:6">
-      <c r="A60" s="3"/>
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
-      <c r="D60"/>
-      <c r="E60" s="6"/>
-      <c r="F60" s="3"/>
+      <c r="A60" s="5"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="5"/>
     </row>
     <row r="61" ht="15" spans="1:6">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="4"/>
-      <c r="D61"/>
-      <c r="E61" s="6"/>
-      <c r="F61" s="3"/>
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="6"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="5"/>
     </row>
     <row r="62" ht="15" spans="1:6">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="4"/>
-      <c r="D62"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="3"/>
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="6"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="5"/>
     </row>
     <row r="63" ht="15" spans="1:6">
-      <c r="A63" s="3"/>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-      <c r="D63"/>
-      <c r="E63" s="6"/>
-      <c r="F63" s="3"/>
+      <c r="A63" s="5"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="5"/>
     </row>
     <row r="64" ht="15" spans="1:6">
-      <c r="A64" s="3"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="4"/>
-      <c r="D64"/>
-      <c r="E64" s="6"/>
-      <c r="F64" s="3"/>
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="6"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="5"/>
     </row>
     <row r="65" ht="15" spans="1:6">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="4"/>
-      <c r="D65"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="3"/>
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="6"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="5"/>
     </row>
     <row r="66" ht="15" spans="1:6">
-      <c r="A66" s="3"/>
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
-      <c r="D66"/>
-      <c r="E66" s="6"/>
-      <c r="F66" s="3"/>
+      <c r="A66" s="5"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="E66" s="8"/>
+      <c r="F66" s="5"/>
     </row>
     <row r="67" ht="15" spans="1:6">
-      <c r="A67" s="3"/>
-      <c r="B67" s="3"/>
-      <c r="C67" s="4"/>
-      <c r="D67"/>
-      <c r="E67" s="6"/>
-      <c r="F67" s="3"/>
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="6"/>
+      <c r="E67" s="8"/>
+      <c r="F67" s="5"/>
     </row>
     <row r="68" ht="15" spans="1:6">
-      <c r="A68" s="3"/>
-      <c r="B68" s="3"/>
-      <c r="C68" s="4"/>
-      <c r="D68"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="3"/>
+      <c r="A68" s="5"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="6"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="5"/>
     </row>
     <row r="69" ht="15" spans="1:6">
-      <c r="A69" s="3"/>
-      <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
-      <c r="D69"/>
-      <c r="E69" s="6"/>
-      <c r="F69" s="3"/>
+      <c r="A69" s="5"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="E69" s="8"/>
+      <c r="F69" s="5"/>
     </row>
     <row r="70" ht="15" spans="1:6">
-      <c r="A70" s="3"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="4"/>
-      <c r="D70"/>
-      <c r="E70" s="6"/>
-      <c r="F70" s="3"/>
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="6"/>
+      <c r="E70" s="8"/>
+      <c r="F70" s="5"/>
     </row>
     <row r="71" ht="15" spans="1:6">
-      <c r="A71" s="3"/>
-      <c r="B71" s="3"/>
-      <c r="C71" s="4"/>
-      <c r="D71"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="3"/>
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="6"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="5"/>
     </row>
     <row r="72" ht="15" spans="1:6">
-      <c r="A72" s="3"/>
-      <c r="B72" s="4"/>
-      <c r="C72" s="4"/>
-      <c r="D72"/>
-      <c r="E72" s="6"/>
-      <c r="F72" s="3"/>
+      <c r="A72" s="5"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="6"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="5"/>
     </row>
     <row r="73" ht="15" spans="1:6">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="4"/>
-      <c r="D73"/>
-      <c r="E73" s="6"/>
-      <c r="F73" s="3"/>
+      <c r="A73" s="5"/>
+      <c r="B73" s="5"/>
+      <c r="C73" s="6"/>
+      <c r="E73" s="8"/>
+      <c r="F73" s="5"/>
     </row>
     <row r="74" ht="15" spans="1:6">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="4"/>
-      <c r="D74"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="3"/>
+      <c r="A74" s="5"/>
+      <c r="B74" s="5"/>
+      <c r="C74" s="6"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="5"/>
     </row>
     <row r="75" ht="15" spans="1:6">
-      <c r="A75" s="3"/>
-      <c r="B75" s="4"/>
-      <c r="C75" s="4"/>
-      <c r="D75"/>
-      <c r="E75" s="6"/>
-      <c r="F75" s="3"/>
+      <c r="A75" s="5"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="E75" s="8"/>
+      <c r="F75" s="5"/>
     </row>
     <row r="76" ht="15" spans="1:6">
-      <c r="A76" s="3"/>
-      <c r="B76" s="3"/>
-      <c r="C76" s="4"/>
-      <c r="D76"/>
-      <c r="E76" s="6"/>
-      <c r="F76" s="3"/>
+      <c r="A76" s="5"/>
+      <c r="B76" s="5"/>
+      <c r="C76" s="6"/>
+      <c r="E76" s="8"/>
+      <c r="F76" s="5"/>
     </row>
     <row r="77" ht="15" spans="1:6">
-      <c r="A77" s="3"/>
-      <c r="B77" s="3"/>
-      <c r="C77" s="4"/>
-      <c r="D77"/>
-      <c r="E77" s="5"/>
-      <c r="F77" s="3"/>
+      <c r="A77" s="5"/>
+      <c r="B77" s="5"/>
+      <c r="C77" s="6"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="5"/>
     </row>
     <row r="78" ht="15" spans="1:6">
-      <c r="A78" s="3"/>
-      <c r="B78" s="4"/>
-      <c r="C78" s="4"/>
-      <c r="D78"/>
-      <c r="E78" s="6"/>
-      <c r="F78" s="3"/>
+      <c r="A78" s="5"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="E78" s="8"/>
+      <c r="F78" s="5"/>
     </row>
     <row r="79" ht="15" spans="1:6">
-      <c r="A79" s="3"/>
-      <c r="B79" s="3"/>
-      <c r="C79" s="4"/>
-      <c r="D79"/>
-      <c r="E79" s="6"/>
-      <c r="F79" s="3"/>
+      <c r="A79" s="5"/>
+      <c r="B79" s="5"/>
+      <c r="C79" s="6"/>
+      <c r="E79" s="8"/>
+      <c r="F79" s="5"/>
     </row>
     <row r="80" ht="15" spans="1:6">
-      <c r="A80" s="3"/>
-      <c r="B80" s="3"/>
-      <c r="C80" s="4"/>
-      <c r="D80"/>
-      <c r="E80" s="5"/>
-      <c r="F80" s="3"/>
+      <c r="A80" s="5"/>
+      <c r="B80" s="5"/>
+      <c r="C80" s="6"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="5"/>
     </row>
     <row r="81" ht="15" spans="1:6">
-      <c r="A81" s="3"/>
-      <c r="B81" s="4"/>
-      <c r="C81" s="4"/>
-      <c r="D81"/>
-      <c r="E81" s="6"/>
-      <c r="F81" s="3"/>
+      <c r="A81" s="5"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="6"/>
+      <c r="E81" s="8"/>
+      <c r="F81" s="5"/>
     </row>
     <row r="82" ht="15" spans="1:6">
-      <c r="A82" s="3"/>
-      <c r="B82" s="3"/>
-      <c r="C82" s="4"/>
-      <c r="D82"/>
-      <c r="E82" s="6"/>
-      <c r="F82" s="3"/>
+      <c r="A82" s="5"/>
+      <c r="B82" s="5"/>
+      <c r="C82" s="6"/>
+      <c r="E82" s="8"/>
+      <c r="F82" s="5"/>
     </row>
     <row r="83" ht="15" spans="1:6">
-      <c r="A83" s="3"/>
-      <c r="B83" s="3"/>
-      <c r="C83" s="4"/>
-      <c r="D83"/>
-      <c r="E83" s="5"/>
-      <c r="F83" s="3"/>
+      <c r="A83" s="5"/>
+      <c r="B83" s="5"/>
+      <c r="C83" s="6"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="5"/>
     </row>
     <row r="84" ht="15" spans="1:6">
-      <c r="A84" s="3"/>
-      <c r="B84" s="4"/>
-      <c r="C84" s="4"/>
-      <c r="D84"/>
-      <c r="E84" s="6"/>
-      <c r="F84" s="3"/>
+      <c r="A84" s="5"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
+      <c r="E84" s="8"/>
+      <c r="F84" s="5"/>
     </row>
     <row r="85" ht="15" spans="1:6">
-      <c r="A85" s="3"/>
-      <c r="B85" s="3"/>
-      <c r="C85" s="4"/>
-      <c r="D85"/>
-      <c r="E85" s="6"/>
-      <c r="F85" s="3"/>
+      <c r="A85" s="5"/>
+      <c r="B85" s="5"/>
+      <c r="C85" s="6"/>
+      <c r="E85" s="8"/>
+      <c r="F85" s="5"/>
     </row>
     <row r="86" ht="15" spans="1:6">
-      <c r="A86" s="3"/>
-      <c r="B86" s="3"/>
-      <c r="C86" s="4"/>
-      <c r="D86"/>
-      <c r="E86" s="5"/>
-      <c r="F86" s="3"/>
+      <c r="A86" s="5"/>
+      <c r="B86" s="5"/>
+      <c r="C86" s="6"/>
+      <c r="E86" s="7"/>
+      <c r="F86" s="5"/>
     </row>
     <row r="87" ht="15" spans="1:6">
-      <c r="A87" s="3"/>
-      <c r="B87" s="4"/>
-      <c r="C87" s="4"/>
-      <c r="D87"/>
-      <c r="E87" s="6"/>
-      <c r="F87" s="3"/>
+      <c r="A87" s="5"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="6"/>
+      <c r="E87" s="8"/>
+      <c r="F87" s="5"/>
     </row>
     <row r="88" ht="15" spans="1:6">
-      <c r="A88" s="3"/>
-      <c r="B88" s="3"/>
-      <c r="C88" s="4"/>
-      <c r="D88"/>
-      <c r="E88" s="6"/>
-      <c r="F88" s="3"/>
+      <c r="A88" s="5"/>
+      <c r="B88" s="5"/>
+      <c r="C88" s="6"/>
+      <c r="E88" s="8"/>
+      <c r="F88" s="5"/>
     </row>
     <row r="89" ht="15" spans="1:6">
-      <c r="A89" s="3"/>
-      <c r="B89" s="3"/>
-      <c r="C89" s="4"/>
-      <c r="D89"/>
-      <c r="E89" s="5"/>
-      <c r="F89" s="3"/>
+      <c r="A89" s="5"/>
+      <c r="B89" s="5"/>
+      <c r="C89" s="6"/>
+      <c r="E89" s="7"/>
+      <c r="F89" s="5"/>
     </row>
     <row r="90" ht="15" spans="1:6">
-      <c r="A90" s="3"/>
-      <c r="B90" s="4"/>
-      <c r="C90" s="4"/>
-      <c r="D90"/>
-      <c r="E90" s="6"/>
-      <c r="F90" s="3"/>
+      <c r="A90" s="5"/>
+      <c r="B90" s="6"/>
+      <c r="C90" s="6"/>
+      <c r="E90" s="8"/>
+      <c r="F90" s="5"/>
     </row>
     <row r="91" ht="15" spans="1:6">
-      <c r="A91" s="3"/>
-      <c r="B91" s="3"/>
-      <c r="C91" s="4"/>
-      <c r="D91"/>
-      <c r="E91" s="6"/>
-      <c r="F91" s="3"/>
+      <c r="A91" s="5"/>
+      <c r="B91" s="5"/>
+      <c r="C91" s="6"/>
+      <c r="E91" s="8"/>
+      <c r="F91" s="5"/>
     </row>
     <row r="92" ht="15" spans="1:6">
-      <c r="A92" s="3"/>
-      <c r="B92" s="3"/>
-      <c r="C92" s="4"/>
-      <c r="D92"/>
-      <c r="E92" s="5"/>
-      <c r="F92" s="3"/>
+      <c r="A92" s="5"/>
+      <c r="B92" s="5"/>
+      <c r="C92" s="6"/>
+      <c r="E92" s="7"/>
+      <c r="F92" s="5"/>
     </row>
     <row r="93" ht="15" spans="1:6">
-      <c r="A93" s="3"/>
-      <c r="B93" s="4"/>
-      <c r="C93" s="4"/>
-      <c r="D93"/>
-      <c r="E93" s="6"/>
-      <c r="F93" s="3"/>
+      <c r="A93" s="5"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="6"/>
+      <c r="E93" s="8"/>
+      <c r="F93" s="5"/>
     </row>
     <row r="94" ht="15" spans="1:6">
-      <c r="A94" s="3"/>
-      <c r="B94" s="3"/>
-      <c r="C94" s="4"/>
-      <c r="D94"/>
-      <c r="E94" s="6"/>
-      <c r="F94" s="3"/>
+      <c r="A94" s="5"/>
+      <c r="B94" s="5"/>
+      <c r="C94" s="6"/>
+      <c r="E94" s="8"/>
+      <c r="F94" s="5"/>
     </row>
     <row r="95" ht="15" spans="1:6">
-      <c r="A95" s="3"/>
-      <c r="B95" s="3"/>
-      <c r="C95" s="4"/>
-      <c r="D95"/>
-      <c r="E95" s="5"/>
-      <c r="F95" s="3"/>
+      <c r="A95" s="5"/>
+      <c r="B95" s="5"/>
+      <c r="C95" s="6"/>
+      <c r="E95" s="7"/>
+      <c r="F95" s="5"/>
     </row>
     <row r="96" ht="15" spans="1:6">
-      <c r="A96" s="3"/>
-      <c r="B96" s="4"/>
-      <c r="C96" s="4"/>
-      <c r="D96"/>
-      <c r="E96" s="6"/>
-      <c r="F96" s="3"/>
+      <c r="A96" s="5"/>
+      <c r="B96" s="6"/>
+      <c r="C96" s="6"/>
+      <c r="E96" s="8"/>
+      <c r="F96" s="5"/>
     </row>
     <row r="97" ht="15" spans="1:6">
-      <c r="A97" s="3"/>
-      <c r="B97" s="3"/>
-      <c r="C97" s="4"/>
-      <c r="D97"/>
-      <c r="E97" s="6"/>
-      <c r="F97" s="3"/>
+      <c r="A97" s="5"/>
+      <c r="B97" s="5"/>
+      <c r="C97" s="6"/>
+      <c r="E97" s="8"/>
+      <c r="F97" s="5"/>
     </row>
     <row r="98" ht="15" spans="1:6">
-      <c r="A98" s="3"/>
-      <c r="B98" s="3"/>
-      <c r="C98" s="4"/>
-      <c r="D98"/>
-      <c r="E98" s="5"/>
-      <c r="F98" s="3"/>
+      <c r="A98" s="5"/>
+      <c r="B98" s="5"/>
+      <c r="C98" s="6"/>
+      <c r="E98" s="7"/>
+      <c r="F98" s="5"/>
     </row>
     <row r="99" ht="15" spans="1:6">
-      <c r="A99" s="3"/>
-      <c r="B99" s="4"/>
-      <c r="C99" s="4"/>
-      <c r="D99"/>
-      <c r="E99" s="6"/>
-      <c r="F99" s="3"/>
+      <c r="A99" s="5"/>
+      <c r="B99" s="6"/>
+      <c r="C99" s="6"/>
+      <c r="E99" s="8"/>
+      <c r="F99" s="5"/>
     </row>
     <row r="100" ht="15" spans="1:6">
-      <c r="A100" s="3"/>
-      <c r="B100" s="3"/>
-      <c r="C100" s="4"/>
-      <c r="D100"/>
-      <c r="E100" s="6"/>
-      <c r="F100" s="3"/>
+      <c r="A100" s="5"/>
+      <c r="B100" s="5"/>
+      <c r="C100" s="6"/>
+      <c r="E100" s="8"/>
+      <c r="F100" s="5"/>
     </row>
     <row r="101" ht="15" spans="1:6">
-      <c r="A101" s="3"/>
-      <c r="B101" s="3"/>
-      <c r="C101" s="4"/>
-      <c r="D101"/>
-      <c r="E101" s="5"/>
-      <c r="F101" s="3"/>
+      <c r="A101" s="5"/>
+      <c r="B101" s="5"/>
+      <c r="C101" s="6"/>
+      <c r="E101" s="7"/>
+      <c r="F101" s="5"/>
     </row>
     <row r="102" ht="15" spans="1:6">
-      <c r="A102" s="3"/>
-      <c r="B102" s="4"/>
-      <c r="C102" s="4"/>
-      <c r="D102"/>
-      <c r="E102" s="6"/>
-      <c r="F102" s="3"/>
+      <c r="A102" s="5"/>
+      <c r="B102" s="6"/>
+      <c r="C102" s="6"/>
+      <c r="E102" s="8"/>
+      <c r="F102" s="5"/>
     </row>
     <row r="103" ht="15" spans="1:6">
-      <c r="A103" s="3"/>
-      <c r="B103" s="3"/>
-      <c r="C103" s="4"/>
-      <c r="D103"/>
-      <c r="E103" s="6"/>
-      <c r="F103" s="3"/>
+      <c r="A103" s="5"/>
+      <c r="B103" s="5"/>
+      <c r="C103" s="6"/>
+      <c r="E103" s="8"/>
+      <c r="F103" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2256,24 +2250,24 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.9" spans="1:4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:4">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C2" t="s">
@@ -2294,8 +2288,8 @@
   <sheetPr/>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="7" outlineLevelCol="5"/>
@@ -2304,22 +2298,22 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.9" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2327,20 +2321,20 @@
       <c r="A2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D2" t="str">
         <f>_xlfn.CONCAT(A2,".",B2,"@gmail.com")</f>
         <v>Anil.Sharma@gmail.com</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2348,20 +2342,20 @@
       <c r="A3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D3" t="str">
         <f>_xlfn.CONCAT(A3,".",B3,"@gmail.com")</f>
         <v>Sneha.Gupta@gmail.com</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2369,70 +2363,164 @@
       <c r="A4" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="6" t="s">
         <v>43</v>
       </c>
       <c r="D4" t="str">
         <f>_xlfn.CONCAT(A4,".",B4,"@gmail.com")</f>
         <v>Rohan.Sen@gmail.com</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" ht="15" spans="1:6">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="6" t="s">
         <v>47</v>
       </c>
       <c r="D5" t="str">
         <f>_xlfn.CONCAT(A5,".",B5,"@gmail.com")</f>
         <v>Aditi.Chakrabotry@gmail.com</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="6" ht="15" spans="1:6">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="3"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" ht="15" spans="1:6">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="3"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" ht="15" spans="1:6">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="3"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="15.2222222222222" customWidth="1"/>
+    <col min="2" max="2" width="15.7777777777778" customWidth="1"/>
+    <col min="3" max="3" width="21.8888888888889" customWidth="1"/>
+    <col min="4" max="4" width="19.1111111111111" customWidth="1"/>
+    <col min="5" max="5" width="25.2222222222222" customWidth="1"/>
+    <col min="6" max="6" width="13.7777777777778" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3">
+        <v>254</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>